<commit_message>
to create a table use by bootstrap
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>张冠鹏</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -32,22 +33,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>单位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>专长</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>职务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>孙家盼</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -125,6 +110,22 @@
   </si>
   <si>
     <t>沙瑞金</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>department</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>speciality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>job</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -476,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -488,16 +489,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -516,86 +517,173 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create the table in myself method
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>张冠鹏</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -126,6 +126,14 @@
   </si>
   <si>
     <t>job</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jobTitle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -608,81 +616,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish the talbe creating
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -129,11 +129,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>jobTitle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jobTitle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -619,7 +619,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -630,7 +630,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
@@ -642,7 +642,7 @@
         <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add the Scrollable to the dataTable
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="48">
   <si>
     <t>张冠鹏</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,6 +134,78 @@
   </si>
   <si>
     <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>季昌明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汉东大学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检查</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检察长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陆亦可</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汉东大学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>侦查</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>侦查处长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>林华华</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检查</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>美女科长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周正</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汉东大学政法系2009级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>科长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高玉亮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汉东大学政法系1990级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>政法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>政法委书记</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -483,15 +555,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="2" max="2" width="21.375" customWidth="1"/>
     <col min="3" max="3" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -605,6 +677,244 @@
       </c>
       <c r="D8" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>